<commit_message>
Updated to include EFG T4.4a.
</commit_message>
<xml_diff>
--- a/crosswalks/NVIS-IUCNGET/Terrestrial_IUCNGET.xlsx
+++ b/crosswalks/NVIS-IUCNGET/Terrestrial_IUCNGET.xlsx
@@ -5,39 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/new298_csiro_au/Documents/Code/Python/NEAP/ecosystem-typology/crosswalks/NVIS-IUCNGET/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fishe\Dropbox\Documents\NEAP\Ecosystem-Typology\crosswalks\NVIS-IUCNGET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="13_ncr:1_{643A7B15-3DDC-4E8D-8046-3F097D81BDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{025056E4-D196-4787-AF9B-96363E7D5B18}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC73AB4F-EDBC-48AA-BE79-6AA1A75134AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3315" yWindow="840" windowWidth="21600" windowHeight="11430" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="11" r:id="rId1"/>
     <sheet name="SSSOM" sheetId="18" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="289">
   <si>
     <t>MFT1.3 Coastal saltmarshes and reedbeds</t>
   </si>
@@ -913,10 +902,10 @@
     <t>terr:T4.4a_Semi_arid_woodlands</t>
   </si>
   <si>
-    <t>skos:narrowMatch</t>
-  </si>
-  <si>
     <t>low</t>
+  </si>
+  <si>
+    <t>get:groups/T4.4a</t>
   </si>
 </sst>
 </file>
@@ -1047,9 +1036,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1087,7 +1076,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1193,7 +1182,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1335,7 +1324,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1416,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564BC65A-26C0-42CC-8916-F0F3B4195637}">
-  <dimension ref="A1:Q75"/>
+  <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="B70" sqref="A70:XFD75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3695,13 +3684,13 @@
         <v>285</v>
       </c>
       <c r="C69" t="s">
-        <v>287</v>
+        <v>9</v>
       </c>
       <c r="D69" t="s">
-        <v>172</v>
+        <v>288</v>
       </c>
       <c r="E69" t="s">
-        <v>36</v>
+        <v>285</v>
       </c>
       <c r="F69" t="s">
         <v>8</v>
@@ -3716,219 +3705,9 @@
         <v>45474</v>
       </c>
       <c r="J69" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K69" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>286</v>
-      </c>
-      <c r="B70" t="s">
-        <v>285</v>
-      </c>
-      <c r="C70" t="s">
-        <v>287</v>
-      </c>
-      <c r="D70" t="s">
-        <v>174</v>
-      </c>
-      <c r="E70" t="s">
-        <v>38</v>
-      </c>
-      <c r="F70" t="s">
-        <v>8</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="H70" t="s">
-        <v>194</v>
-      </c>
-      <c r="I70" s="4">
-        <v>45474</v>
-      </c>
-      <c r="J70" t="s">
-        <v>288</v>
-      </c>
-      <c r="K70" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>286</v>
-      </c>
-      <c r="B71" t="s">
-        <v>285</v>
-      </c>
-      <c r="C71" t="s">
-        <v>287</v>
-      </c>
-      <c r="D71" t="s">
-        <v>175</v>
-      </c>
-      <c r="E71" t="s">
-        <v>40</v>
-      </c>
-      <c r="F71" t="s">
-        <v>8</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="H71" t="s">
-        <v>194</v>
-      </c>
-      <c r="I71" s="4">
-        <v>45474</v>
-      </c>
-      <c r="J71" t="s">
-        <v>288</v>
-      </c>
-      <c r="K71" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>286</v>
-      </c>
-      <c r="B72" t="s">
-        <v>285</v>
-      </c>
-      <c r="C72" t="s">
-        <v>287</v>
-      </c>
-      <c r="D72" t="s">
-        <v>176</v>
-      </c>
-      <c r="E72" t="s">
-        <v>41</v>
-      </c>
-      <c r="F72" t="s">
-        <v>8</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="H72" t="s">
-        <v>194</v>
-      </c>
-      <c r="I72" s="4">
-        <v>45474</v>
-      </c>
-      <c r="J72" t="s">
-        <v>288</v>
-      </c>
-      <c r="K72" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>286</v>
-      </c>
-      <c r="B73" t="s">
-        <v>285</v>
-      </c>
-      <c r="C73" t="s">
-        <v>287</v>
-      </c>
-      <c r="D73" t="s">
-        <v>177</v>
-      </c>
-      <c r="E73" t="s">
-        <v>39</v>
-      </c>
-      <c r="F73" t="s">
-        <v>8</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="H73" t="s">
-        <v>194</v>
-      </c>
-      <c r="I73" s="4">
-        <v>45474</v>
-      </c>
-      <c r="J73" t="s">
-        <v>288</v>
-      </c>
-      <c r="K73" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>286</v>
-      </c>
-      <c r="B74" t="s">
-        <v>285</v>
-      </c>
-      <c r="C74" t="s">
-        <v>287</v>
-      </c>
-      <c r="D74" t="s">
-        <v>179</v>
-      </c>
-      <c r="E74" t="s">
-        <v>44</v>
-      </c>
-      <c r="F74" t="s">
-        <v>8</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="H74" t="s">
-        <v>194</v>
-      </c>
-      <c r="I74" s="4">
-        <v>45474</v>
-      </c>
-      <c r="J74" t="s">
-        <v>288</v>
-      </c>
-      <c r="K74" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>286</v>
-      </c>
-      <c r="B75" t="s">
-        <v>285</v>
-      </c>
-      <c r="C75" t="s">
-        <v>287</v>
-      </c>
-      <c r="D75" t="s">
-        <v>180</v>
-      </c>
-      <c r="E75" t="s">
-        <v>43</v>
-      </c>
-      <c r="F75" t="s">
-        <v>8</v>
-      </c>
-      <c r="G75" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="H75" t="s">
-        <v>194</v>
-      </c>
-      <c r="I75" s="4">
-        <v>45474</v>
-      </c>
-      <c r="J75" t="s">
-        <v>288</v>
-      </c>
-      <c r="K75" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3939,65 +3718,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
+    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
+    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
+      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
+      <Description>63P7TJYCZHM3-28990658-16955</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -4273,40 +4010,77 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
-    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
-    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
-      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
-      <Description>63P7TJYCZHM3-28990658-16955</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
+    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4325,13 +4099,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
-    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add T2.1, TF1.1, and TF1.7
</commit_message>
<xml_diff>
--- a/crosswalks/NVIS-IUCNGET/Terrestrial_IUCNGET.xlsx
+++ b/crosswalks/NVIS-IUCNGET/Terrestrial_IUCNGET.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fishe\Dropbox\Documents\NEAP\Ecosystem-Typology\crosswalks\NVIS-IUCNGET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu240\Downloads\ext\ecosystem-typology\crosswalks\NVIS-IUCNGET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFE62FF-0116-43FE-B231-E09279DE5894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29866265-5787-4BD4-80E4-81382AEEE962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="11" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="297">
   <si>
     <t>MFT1.3 Coastal saltmarshes and reedbeds</t>
   </si>
@@ -908,12 +908,36 @@
   <si>
     <t>get:groups/T4.4a</t>
   </si>
+  <si>
+    <t>get:groups/T2.1</t>
+  </si>
+  <si>
+    <t>T2.1 Boreal and temperate high montane forests and woodlands</t>
+  </si>
+  <si>
+    <t>get:groups/TF1.1</t>
+  </si>
+  <si>
+    <t>TF1.1 Tropical flooded forests and peat forests</t>
+  </si>
+  <si>
+    <t>TF1.7 Boreal and temperate fens</t>
+  </si>
+  <si>
+    <t>get:groups/TF1.7</t>
+  </si>
+  <si>
+    <t>orcid:0000-0003-0956-3208</t>
+  </si>
+  <si>
+    <t>Ning Liu</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -982,6 +1006,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1006,7 +1036,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
@@ -1016,6 +1046,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink 2" xfId="1" xr:uid="{056D7D6A-1EC3-49F3-966A-4D5DDECD64D3}"/>
@@ -1037,9 +1068,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1077,7 +1108,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1183,7 +1214,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1325,7 +1356,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1339,62 +1370,62 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="104.140625" customWidth="1"/>
+    <col min="1" max="1" width="104.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -1406,33 +1437,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564BC65A-26C0-42CC-8916-F0F3B4195637}">
-  <dimension ref="A1:Q69"/>
+  <dimension ref="A1:Q72"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E69" sqref="E2:E69"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61:I61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="50.140625" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="50.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="50.1796875" customWidth="1"/>
+    <col min="6" max="6" width="29.1796875" customWidth="1"/>
     <col min="7" max="8" width="34" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.7265625" customWidth="1"/>
+    <col min="10" max="10" width="9.453125" customWidth="1"/>
+    <col min="11" max="11" width="15.453125" customWidth="1"/>
     <col min="12" max="12" width="34" customWidth="1"/>
-    <col min="13" max="13" width="35.85546875" customWidth="1"/>
-    <col min="14" max="14" width="34.42578125" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.85546875" customWidth="1"/>
-    <col min="17" max="17" width="57.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.81640625" customWidth="1"/>
+    <col min="14" max="14" width="34.453125" customWidth="1"/>
+    <col min="15" max="15" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.81640625" customWidth="1"/>
+    <col min="17" max="17" width="57.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>68</v>
       </c>
@@ -1481,7 +1512,7 @@
       <c r="P1" s="5"/>
       <c r="Q1"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -1515,7 +1546,7 @@
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -1549,7 +1580,7 @@
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -1583,7 +1614,7 @@
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1617,7 +1648,7 @@
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1651,7 +1682,7 @@
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>88</v>
       </c>
@@ -1684,7 +1715,7 @@
       </c>
       <c r="P7" s="3"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>89</v>
       </c>
@@ -1717,7 +1748,7 @@
       </c>
       <c r="P8" s="3"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>90</v>
       </c>
@@ -1750,7 +1781,7 @@
       </c>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>91</v>
       </c>
@@ -1783,7 +1814,7 @@
       </c>
       <c r="P10" s="3"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>282</v>
       </c>
@@ -1816,7 +1847,7 @@
       </c>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>92</v>
       </c>
@@ -1849,7 +1880,7 @@
       </c>
       <c r="P12" s="3"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -1882,7 +1913,7 @@
       </c>
       <c r="P13" s="3"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -1915,7 +1946,7 @@
       </c>
       <c r="P14" s="3"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -1948,7 +1979,7 @@
       </c>
       <c r="P15" s="3"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>96</v>
       </c>
@@ -1981,7 +2012,7 @@
       </c>
       <c r="P16" s="3"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>97</v>
       </c>
@@ -2014,7 +2045,7 @@
       </c>
       <c r="P17" s="3"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>98</v>
       </c>
@@ -2047,7 +2078,7 @@
       </c>
       <c r="P18" s="3"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2080,7 +2111,7 @@
       </c>
       <c r="P19" s="3"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -2113,7 +2144,7 @@
       </c>
       <c r="P20" s="3"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -2146,7 +2177,7 @@
       </c>
       <c r="P21" s="3"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -2179,7 +2210,7 @@
       </c>
       <c r="P22" s="3"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -2212,7 +2243,7 @@
       </c>
       <c r="P23" s="3"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -2245,7 +2276,7 @@
       </c>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -2278,7 +2309,7 @@
       </c>
       <c r="P25" s="3"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>106</v>
       </c>
@@ -2311,7 +2342,7 @@
       </c>
       <c r="P26" s="3"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -2344,7 +2375,7 @@
       </c>
       <c r="P27" s="3"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -2377,7 +2408,7 @@
       </c>
       <c r="P28" s="3"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>109</v>
       </c>
@@ -2410,7 +2441,7 @@
       </c>
       <c r="P29" s="3"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>283</v>
       </c>
@@ -2443,7 +2474,7 @@
       </c>
       <c r="P30" s="3"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -2476,7 +2507,7 @@
       </c>
       <c r="P31" s="3"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>111</v>
       </c>
@@ -2509,7 +2540,7 @@
       </c>
       <c r="P32" s="3"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>112</v>
       </c>
@@ -2542,7 +2573,7 @@
       </c>
       <c r="P33" s="3"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>113</v>
       </c>
@@ -2575,771 +2606,766 @@
       </c>
       <c r="P34" s="3"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B35" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>289</v>
+      </c>
+      <c r="E35" t="s">
+        <v>290</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="H35" t="s">
+        <v>296</v>
+      </c>
+      <c r="I35" s="4">
+        <v>45504</v>
+      </c>
+      <c r="K35" t="s">
+        <v>66</v>
+      </c>
+      <c r="P35" s="3"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>114</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>33</v>
       </c>
-      <c r="C35" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
         <v>169</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E36" t="s">
         <v>33</v>
       </c>
-      <c r="F35" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" s="3" t="s">
+      <c r="F36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="H35" t="s">
-        <v>194</v>
-      </c>
-      <c r="I35" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K35" t="s">
-        <v>66</v>
-      </c>
-      <c r="P35" s="3"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="H36" t="s">
+        <v>194</v>
+      </c>
+      <c r="I36" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K36" t="s">
+        <v>66</v>
+      </c>
+      <c r="P36" s="3"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>115</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>34</v>
       </c>
-      <c r="C36" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" t="s">
         <v>170</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>34</v>
       </c>
-      <c r="F36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" s="3" t="s">
+      <c r="F37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="H36" t="s">
-        <v>194</v>
-      </c>
-      <c r="I36" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K36" t="s">
-        <v>66</v>
-      </c>
-      <c r="P36" s="3"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="H37" t="s">
+        <v>194</v>
+      </c>
+      <c r="I37" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K37" t="s">
+        <v>66</v>
+      </c>
+      <c r="P37" s="3"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>116</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>35</v>
       </c>
-      <c r="C37" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s">
         <v>171</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>35</v>
       </c>
-      <c r="F37" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="3" t="s">
+      <c r="F38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="H37" t="s">
-        <v>194</v>
-      </c>
-      <c r="I37" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K37" t="s">
-        <v>66</v>
-      </c>
-      <c r="P37" s="3"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="H38" t="s">
+        <v>194</v>
+      </c>
+      <c r="I38" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K38" t="s">
+        <v>66</v>
+      </c>
+      <c r="P38" s="3"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>117</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>36</v>
       </c>
-      <c r="C38" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" t="s">
         <v>172</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>36</v>
       </c>
-      <c r="F38" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="3" t="s">
+      <c r="F39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="H38" t="s">
-        <v>194</v>
-      </c>
-      <c r="I38" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K38" t="s">
-        <v>66</v>
-      </c>
-      <c r="P38" s="3"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="H39" t="s">
+        <v>194</v>
+      </c>
+      <c r="I39" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K39" t="s">
+        <v>66</v>
+      </c>
+      <c r="P39" s="3"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>118</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>37</v>
       </c>
-      <c r="C39" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" t="s">
         <v>173</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E40" t="s">
         <v>37</v>
       </c>
-      <c r="F39" t="s">
-        <v>8</v>
-      </c>
-      <c r="G39" s="3" t="s">
+      <c r="F40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="H39" t="s">
-        <v>194</v>
-      </c>
-      <c r="I39" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K39" t="s">
-        <v>66</v>
-      </c>
-      <c r="P39" s="3"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="H40" t="s">
+        <v>194</v>
+      </c>
+      <c r="I40" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K40" t="s">
+        <v>66</v>
+      </c>
+      <c r="P40" s="3"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>119</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>38</v>
       </c>
-      <c r="C40" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" t="s">
         <v>174</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>38</v>
       </c>
-      <c r="F40" t="s">
-        <v>8</v>
-      </c>
-      <c r="G40" s="3" t="s">
+      <c r="F41" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="H40" t="s">
-        <v>194</v>
-      </c>
-      <c r="I40" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K40" t="s">
-        <v>66</v>
-      </c>
-      <c r="P40" s="3"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="H41" t="s">
+        <v>194</v>
+      </c>
+      <c r="I41" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K41" t="s">
+        <v>66</v>
+      </c>
+      <c r="P41" s="3"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>120</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>40</v>
       </c>
-      <c r="C41" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" t="s">
         <v>175</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E42" t="s">
         <v>40</v>
       </c>
-      <c r="F41" t="s">
-        <v>8</v>
-      </c>
-      <c r="G41" s="3" t="s">
+      <c r="F42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="H41" t="s">
-        <v>194</v>
-      </c>
-      <c r="I41" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K41" t="s">
-        <v>66</v>
-      </c>
-      <c r="P41" s="3"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="H42" t="s">
+        <v>194</v>
+      </c>
+      <c r="I42" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K42" t="s">
+        <v>66</v>
+      </c>
+      <c r="P42" s="3"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>121</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>41</v>
       </c>
-      <c r="C42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s">
         <v>176</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E43" t="s">
         <v>41</v>
       </c>
-      <c r="F42" t="s">
-        <v>8</v>
-      </c>
-      <c r="G42" s="3" t="s">
+      <c r="F43" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="H42" t="s">
-        <v>194</v>
-      </c>
-      <c r="I42" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K42" t="s">
-        <v>66</v>
-      </c>
-      <c r="P42" s="3"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="H43" t="s">
+        <v>194</v>
+      </c>
+      <c r="I43" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K43" t="s">
+        <v>66</v>
+      </c>
+      <c r="P43" s="3"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>122</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>39</v>
       </c>
-      <c r="C43" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" t="s">
         <v>177</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E44" t="s">
         <v>39</v>
       </c>
-      <c r="F43" t="s">
-        <v>8</v>
-      </c>
-      <c r="G43" s="3" t="s">
+      <c r="F44" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="H43" t="s">
-        <v>194</v>
-      </c>
-      <c r="I43" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K43" t="s">
-        <v>66</v>
-      </c>
-      <c r="P43" s="3"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="H44" t="s">
+        <v>194</v>
+      </c>
+      <c r="I44" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K44" t="s">
+        <v>66</v>
+      </c>
+      <c r="P44" s="3"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>123</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>42</v>
       </c>
-      <c r="C44" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="C45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" t="s">
         <v>178</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E45" t="s">
         <v>42</v>
       </c>
-      <c r="F44" t="s">
-        <v>8</v>
-      </c>
-      <c r="G44" s="3" t="s">
+      <c r="F45" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="H44" t="s">
-        <v>194</v>
-      </c>
-      <c r="I44" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K44" t="s">
-        <v>66</v>
-      </c>
-      <c r="P44" s="3"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="H45" t="s">
+        <v>194</v>
+      </c>
+      <c r="I45" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K45" t="s">
+        <v>66</v>
+      </c>
+      <c r="P45" s="3"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>124</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>44</v>
       </c>
-      <c r="C45" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="C46" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" t="s">
         <v>179</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E46" t="s">
         <v>44</v>
       </c>
-      <c r="F45" t="s">
-        <v>8</v>
-      </c>
-      <c r="G45" s="3" t="s">
+      <c r="F46" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="H45" t="s">
-        <v>194</v>
-      </c>
-      <c r="I45" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K45" t="s">
-        <v>66</v>
-      </c>
-      <c r="P45" s="3"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="H46" t="s">
+        <v>194</v>
+      </c>
+      <c r="I46" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K46" t="s">
+        <v>66</v>
+      </c>
+      <c r="P46" s="3"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>125</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>43</v>
       </c>
-      <c r="C46" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
         <v>180</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E47" t="s">
         <v>43</v>
       </c>
-      <c r="F46" t="s">
-        <v>8</v>
-      </c>
-      <c r="G46" s="3" t="s">
+      <c r="F47" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="H46" t="s">
-        <v>194</v>
-      </c>
-      <c r="I46" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K46" t="s">
-        <v>66</v>
-      </c>
-      <c r="P46" s="3"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="H47" t="s">
+        <v>194</v>
+      </c>
+      <c r="I47" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K47" t="s">
+        <v>66</v>
+      </c>
+      <c r="P47" s="3"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>126</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>45</v>
       </c>
-      <c r="C47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" t="s">
         <v>181</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E48" t="s">
         <v>45</v>
       </c>
-      <c r="F47" t="s">
-        <v>8</v>
-      </c>
-      <c r="G47" s="3" t="s">
+      <c r="F48" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="H47" t="s">
-        <v>194</v>
-      </c>
-      <c r="I47" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K47" t="s">
-        <v>66</v>
-      </c>
-      <c r="P47" s="3"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="H48" t="s">
+        <v>194</v>
+      </c>
+      <c r="I48" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K48" t="s">
+        <v>66</v>
+      </c>
+      <c r="P48" s="3"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>127</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>46</v>
       </c>
-      <c r="C48" t="s">
-        <v>9</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" t="s">
         <v>182</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>46</v>
       </c>
-      <c r="F48" t="s">
-        <v>8</v>
-      </c>
-      <c r="G48" s="3" t="s">
+      <c r="F49" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="H48" t="s">
-        <v>194</v>
-      </c>
-      <c r="I48" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K48" t="s">
-        <v>66</v>
-      </c>
-      <c r="P48" s="3"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="H49" t="s">
+        <v>194</v>
+      </c>
+      <c r="I49" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K49" t="s">
+        <v>66</v>
+      </c>
+      <c r="P49" s="3"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>128</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>48</v>
       </c>
-      <c r="C49" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" t="s">
         <v>183</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E50" t="s">
         <v>48</v>
       </c>
-      <c r="F49" t="s">
-        <v>8</v>
-      </c>
-      <c r="G49" s="3" t="s">
+      <c r="F50" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="H49" t="s">
-        <v>194</v>
-      </c>
-      <c r="I49" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K49" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="H50" t="s">
+        <v>194</v>
+      </c>
+      <c r="I50" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K50" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>129</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>49</v>
       </c>
-      <c r="C50" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" t="s">
         <v>184</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E51" t="s">
         <v>49</v>
       </c>
-      <c r="F50" t="s">
-        <v>8</v>
-      </c>
-      <c r="G50" s="3" t="s">
+      <c r="F51" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="H50" t="s">
-        <v>194</v>
-      </c>
-      <c r="I50" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K50" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="H51" t="s">
+        <v>194</v>
+      </c>
+      <c r="I51" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>130</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>50</v>
       </c>
-      <c r="C51" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" t="s">
         <v>185</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E52" t="s">
         <v>50</v>
       </c>
-      <c r="F51" t="s">
-        <v>8</v>
-      </c>
-      <c r="G51" s="3" t="s">
+      <c r="F52" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="H51" t="s">
-        <v>194</v>
-      </c>
-      <c r="I51" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K51" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="H52" t="s">
+        <v>194</v>
+      </c>
+      <c r="I52" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K52" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>131</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>47</v>
       </c>
-      <c r="C52" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" t="s">
         <v>186</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E53" t="s">
         <v>47</v>
       </c>
-      <c r="F52" t="s">
-        <v>8</v>
-      </c>
-      <c r="G52" s="3" t="s">
+      <c r="F53" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="H52" t="s">
-        <v>194</v>
-      </c>
-      <c r="I52" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K52" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="H53" t="s">
+        <v>194</v>
+      </c>
+      <c r="I53" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K53" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>132</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>51</v>
       </c>
-      <c r="C53" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" t="s">
         <v>187</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E54" t="s">
         <v>51</v>
       </c>
-      <c r="F53" t="s">
-        <v>8</v>
-      </c>
-      <c r="G53" s="3" t="s">
+      <c r="F54" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H53" t="s">
-        <v>194</v>
-      </c>
-      <c r="I53" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K53" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="H54" t="s">
+        <v>194</v>
+      </c>
+      <c r="I54" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K54" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B55" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="C55" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" t="s">
+        <v>291</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="F55" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="H55" t="s">
+        <v>296</v>
+      </c>
+      <c r="I55" s="4">
+        <v>45504</v>
+      </c>
+      <c r="K55" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>133</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B56" t="s">
         <v>52</v>
       </c>
-      <c r="C54" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s">
         <v>188</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E56" t="s">
         <v>52</v>
       </c>
-      <c r="F54" t="s">
-        <v>8</v>
-      </c>
-      <c r="G54" s="3" t="s">
+      <c r="F56" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="H54" t="s">
-        <v>194</v>
-      </c>
-      <c r="I54" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K54" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="H56" t="s">
+        <v>194</v>
+      </c>
+      <c r="I56" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K56" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>134</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B57" t="s">
         <v>53</v>
       </c>
-      <c r="C55" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" t="s">
         <v>189</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E57" t="s">
         <v>53</v>
       </c>
-      <c r="F55" t="s">
-        <v>8</v>
-      </c>
-      <c r="G55" s="3" t="s">
+      <c r="F57" t="s">
+        <v>8</v>
+      </c>
+      <c r="G57" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="H55" t="s">
-        <v>194</v>
-      </c>
-      <c r="I55" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K55" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="H57" t="s">
+        <v>194</v>
+      </c>
+      <c r="I57" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K57" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>135</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B58" t="s">
         <v>54</v>
       </c>
-      <c r="C56" t="s">
-        <v>9</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="C58" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" t="s">
         <v>190</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E58" t="s">
         <v>54</v>
-      </c>
-      <c r="F56" t="s">
-        <v>8</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="H56" t="s">
-        <v>194</v>
-      </c>
-      <c r="I56" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K56" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>136</v>
-      </c>
-      <c r="B57" t="s">
-        <v>55</v>
-      </c>
-      <c r="C57" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" t="s">
-        <v>191</v>
-      </c>
-      <c r="E57" t="s">
-        <v>55</v>
-      </c>
-      <c r="F57" t="s">
-        <v>8</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="H57" t="s">
-        <v>194</v>
-      </c>
-      <c r="I57" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K57" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>137</v>
-      </c>
-      <c r="B58" t="s">
-        <v>56</v>
-      </c>
-      <c r="C58" t="s">
-        <v>9</v>
-      </c>
-      <c r="D58" t="s">
-        <v>192</v>
-      </c>
-      <c r="E58" t="s">
-        <v>56</v>
       </c>
       <c r="F58" t="s">
         <v>8</v>
@@ -3357,21 +3383,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>267</v>
+        <v>136</v>
       </c>
       <c r="B59" t="s">
-        <v>249</v>
+        <v>55</v>
       </c>
       <c r="C59" t="s">
         <v>9</v>
       </c>
       <c r="D59" t="s">
-        <v>258</v>
+        <v>191</v>
       </c>
       <c r="E59" t="s">
-        <v>249</v>
+        <v>55</v>
       </c>
       <c r="F59" t="s">
         <v>8</v>
@@ -3389,21 +3415,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>268</v>
+        <v>137</v>
       </c>
       <c r="B60" t="s">
-        <v>251</v>
+        <v>56</v>
       </c>
       <c r="C60" t="s">
         <v>9</v>
       </c>
       <c r="D60" t="s">
-        <v>260</v>
+        <v>192</v>
       </c>
       <c r="E60" t="s">
-        <v>251</v>
+        <v>56</v>
       </c>
       <c r="F60" t="s">
         <v>8</v>
@@ -3421,53 +3447,50 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>269</v>
-      </c>
-      <c r="B61" t="s">
-        <v>252</v>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B61" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="C61" t="s">
         <v>9</v>
       </c>
       <c r="D61" t="s">
-        <v>261</v>
-      </c>
-      <c r="E61" t="s">
-        <v>252</v>
+        <v>294</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="F61" t="s">
         <v>8</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>248</v>
+        <v>295</v>
       </c>
       <c r="H61" t="s">
-        <v>194</v>
+        <v>296</v>
       </c>
       <c r="I61" s="4">
-        <v>45444</v>
+        <v>45504</v>
       </c>
       <c r="K61" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B62" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C62" t="s">
         <v>9</v>
       </c>
       <c r="D62" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E62" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F62" t="s">
         <v>8</v>
@@ -3485,21 +3508,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C63" t="s">
         <v>9</v>
       </c>
       <c r="D63" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F63" t="s">
         <v>8</v>
@@ -3517,21 +3540,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B64" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C64" t="s">
         <v>9</v>
       </c>
       <c r="D64" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E64" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F64" t="s">
         <v>8</v>
@@ -3549,21 +3572,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B65" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C65" t="s">
         <v>9</v>
       </c>
       <c r="D65" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E65" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F65" t="s">
         <v>8</v>
@@ -3581,21 +3604,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B66" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C66" t="s">
         <v>9</v>
       </c>
       <c r="D66" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E66" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F66" t="s">
         <v>8</v>
@@ -3613,21 +3636,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="B67" t="s">
-        <v>278</v>
+        <v>255</v>
       </c>
       <c r="C67" t="s">
         <v>9</v>
       </c>
       <c r="D67" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="E67" t="s">
-        <v>278</v>
+        <v>255</v>
       </c>
       <c r="F67" t="s">
         <v>8</v>
@@ -3645,21 +3668,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B68" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="C68" t="s">
         <v>9</v>
       </c>
       <c r="D68" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="E68" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F68" t="s">
         <v>8</v>
@@ -3677,21 +3700,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="B69" t="s">
-        <v>285</v>
+        <v>257</v>
       </c>
       <c r="C69" t="s">
         <v>9</v>
       </c>
       <c r="D69" t="s">
-        <v>288</v>
+        <v>266</v>
       </c>
       <c r="E69" t="s">
-        <v>285</v>
+        <v>257</v>
       </c>
       <c r="F69" t="s">
         <v>8</v>
@@ -3703,12 +3726,108 @@
         <v>194</v>
       </c>
       <c r="I69" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K69" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>284</v>
+      </c>
+      <c r="B70" t="s">
+        <v>278</v>
+      </c>
+      <c r="C70" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" t="s">
+        <v>281</v>
+      </c>
+      <c r="E70" t="s">
+        <v>278</v>
+      </c>
+      <c r="F70" t="s">
+        <v>8</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="H70" t="s">
+        <v>194</v>
+      </c>
+      <c r="I70" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K70" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>275</v>
+      </c>
+      <c r="B71" t="s">
+        <v>250</v>
+      </c>
+      <c r="C71" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71" t="s">
+        <v>259</v>
+      </c>
+      <c r="E71" t="s">
+        <v>250</v>
+      </c>
+      <c r="F71" t="s">
+        <v>8</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="H71" t="s">
+        <v>194</v>
+      </c>
+      <c r="I71" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K71" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>286</v>
+      </c>
+      <c r="B72" t="s">
+        <v>285</v>
+      </c>
+      <c r="C72" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72" t="s">
+        <v>288</v>
+      </c>
+      <c r="E72" t="s">
+        <v>285</v>
+      </c>
+      <c r="F72" t="s">
+        <v>8</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="H72" t="s">
+        <v>194</v>
+      </c>
+      <c r="I72" s="4">
         <v>45474</v>
       </c>
-      <c r="J69" t="s">
+      <c r="J72" t="s">
         <v>287</v>
       </c>
-      <c r="K69" t="s">
+      <c r="K72" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3722,351 +3841,351 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD4EC6B-F420-4E98-B717-46E4AD07ABBC}">
   <dimension ref="A1:A68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection sqref="A1:A68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>56</v>
       </c>
@@ -4080,65 +4199,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
+    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
+    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
+      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
+      <Description>63P7TJYCZHM3-28990658-16955</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -4414,40 +4491,77 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
-    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
-    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
-      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
-      <Description>63P7TJYCZHM3-28990658-16955</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
+    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4466,13 +4580,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
-    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
revise T4.4a to T5.6 Semi-arid open woodlands
</commit_message>
<xml_diff>
--- a/crosswalks/NVIS-IUCNGET/Terrestrial_IUCNGET.xlsx
+++ b/crosswalks/NVIS-IUCNGET/Terrestrial_IUCNGET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu240\Downloads\ext\ecosystem-typology\crosswalks\NVIS-IUCNGET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29866265-5787-4BD4-80E4-81382AEEE962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3769351C-E611-48DC-B2FA-D40849D7EBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="11" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="296">
   <si>
     <t>MFT1.3 Coastal saltmarshes and reedbeds</t>
   </si>
@@ -897,18 +897,9 @@
     <t>terr:M1.9_Upwelling_zones</t>
   </si>
   <si>
-    <t>T4.4a Semi-arid woodlands</t>
-  </si>
-  <si>
     <t>terr:T4.4a_Semi_arid_woodlands</t>
   </si>
   <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>get:groups/T4.4a</t>
-  </si>
-  <si>
     <t>get:groups/T2.1</t>
   </si>
   <si>
@@ -931,6 +922,12 @@
   </si>
   <si>
     <t>Ning Liu</t>
+  </si>
+  <si>
+    <t>get:groups/T5.6</t>
+  </si>
+  <si>
+    <t>T5.6 Semi-arid open woodlands</t>
   </si>
 </sst>
 </file>
@@ -1439,8 +1436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564BC65A-26C0-42CC-8916-F0F3B4195637}">
   <dimension ref="A1:Q72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61:I61"/>
+    <sheetView topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2608,25 +2605,25 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B35" s="7" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
       </c>
       <c r="D35" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E35" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F35" t="s">
         <v>8</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="H35" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="I35" s="4">
         <v>45504</v>
@@ -3034,58 +3031,57 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>126</v>
+        <v>285</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>295</v>
       </c>
       <c r="C48" t="s">
         <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>181</v>
+        <v>294</v>
       </c>
       <c r="E48" t="s">
-        <v>45</v>
+        <v>295</v>
       </c>
       <c r="F48" t="s">
         <v>8</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>239</v>
+        <v>292</v>
       </c>
       <c r="H48" t="s">
-        <v>194</v>
+        <v>293</v>
       </c>
       <c r="I48" s="4">
-        <v>45444</v>
+        <v>45505</v>
       </c>
       <c r="K48" t="s">
         <v>66</v>
       </c>
-      <c r="P48" s="3"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C49" t="s">
         <v>9</v>
       </c>
       <c r="D49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F49" t="s">
         <v>8</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H49" t="s">
         <v>194</v>
@@ -3100,25 +3096,25 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C50" t="s">
         <v>9</v>
       </c>
       <c r="D50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E50" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F50" t="s">
         <v>8</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H50" t="s">
         <v>194</v>
@@ -3129,28 +3125,29 @@
       <c r="K50" t="s">
         <v>66</v>
       </c>
+      <c r="P50" s="3"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C51" t="s">
         <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F51" t="s">
         <v>8</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H51" t="s">
         <v>194</v>
@@ -3164,25 +3161,25 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C52" t="s">
         <v>9</v>
       </c>
       <c r="D52" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F52" t="s">
         <v>8</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H52" t="s">
         <v>194</v>
@@ -3196,25 +3193,25 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B53" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C53" t="s">
         <v>9</v>
       </c>
       <c r="D53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E53" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F53" t="s">
         <v>8</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H53" t="s">
         <v>194</v>
@@ -3228,92 +3225,92 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
+        <v>131</v>
+      </c>
+      <c r="B54" t="s">
+        <v>47</v>
+      </c>
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" t="s">
+        <v>186</v>
+      </c>
+      <c r="E54" t="s">
+        <v>47</v>
+      </c>
+      <c r="F54" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H54" t="s">
+        <v>194</v>
+      </c>
+      <c r="I54" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K54" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>132</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>51</v>
       </c>
-      <c r="C54" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="C55" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" t="s">
         <v>187</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E55" t="s">
         <v>51</v>
       </c>
-      <c r="F54" t="s">
-        <v>8</v>
-      </c>
-      <c r="G54" s="3" t="s">
+      <c r="F55" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H54" t="s">
-        <v>194</v>
-      </c>
-      <c r="I54" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K54" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B55" s="7" t="s">
+      <c r="H55" t="s">
+        <v>194</v>
+      </c>
+      <c r="I55" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K55" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B56" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s">
+        <v>288</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="F56" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="C55" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" t="s">
-        <v>291</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="F55" t="s">
-        <v>8</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="H55" t="s">
-        <v>296</v>
-      </c>
-      <c r="I55" s="4">
+      <c r="H56" t="s">
+        <v>293</v>
+      </c>
+      <c r="I56" s="4">
         <v>45504</v>
-      </c>
-      <c r="K55" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>133</v>
-      </c>
-      <c r="B56" t="s">
-        <v>52</v>
-      </c>
-      <c r="C56" t="s">
-        <v>9</v>
-      </c>
-      <c r="D56" t="s">
-        <v>188</v>
-      </c>
-      <c r="E56" t="s">
-        <v>52</v>
-      </c>
-      <c r="F56" t="s">
-        <v>8</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H56" t="s">
-        <v>194</v>
-      </c>
-      <c r="I56" s="4">
-        <v>45444</v>
       </c>
       <c r="K56" t="s">
         <v>66</v>
@@ -3321,25 +3318,25 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C57" t="s">
         <v>9</v>
       </c>
       <c r="D57" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F57" t="s">
         <v>8</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H57" t="s">
         <v>194</v>
@@ -3353,25 +3350,25 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C58" t="s">
         <v>9</v>
       </c>
       <c r="D58" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F58" t="s">
         <v>8</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H58" t="s">
         <v>194</v>
@@ -3385,19 +3382,19 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
         <v>9</v>
       </c>
       <c r="D59" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F59" t="s">
         <v>8</v>
@@ -3417,19 +3414,19 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B60" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C60" t="s">
         <v>9</v>
       </c>
       <c r="D60" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E60" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F60" t="s">
         <v>8</v>
@@ -3448,61 +3445,61 @@
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B61" s="7" t="s">
+      <c r="A61" t="s">
+        <v>137</v>
+      </c>
+      <c r="B61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C61" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" t="s">
+        <v>192</v>
+      </c>
+      <c r="E61" t="s">
+        <v>56</v>
+      </c>
+      <c r="F61" t="s">
+        <v>8</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="H61" t="s">
+        <v>194</v>
+      </c>
+      <c r="I61" s="4">
+        <v>45444</v>
+      </c>
+      <c r="K61" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B62" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C62" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" t="s">
+        <v>291</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="F62" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="H62" t="s">
         <v>293</v>
       </c>
-      <c r="C61" t="s">
-        <v>9</v>
-      </c>
-      <c r="D61" t="s">
-        <v>294</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="F61" t="s">
-        <v>8</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="H61" t="s">
-        <v>296</v>
-      </c>
-      <c r="I61" s="4">
+      <c r="I62" s="4">
         <v>45504</v>
-      </c>
-      <c r="K61" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>267</v>
-      </c>
-      <c r="B62" t="s">
-        <v>249</v>
-      </c>
-      <c r="C62" t="s">
-        <v>9</v>
-      </c>
-      <c r="D62" t="s">
-        <v>258</v>
-      </c>
-      <c r="E62" t="s">
-        <v>249</v>
-      </c>
-      <c r="F62" t="s">
-        <v>8</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="H62" t="s">
-        <v>194</v>
-      </c>
-      <c r="I62" s="4">
-        <v>45444</v>
       </c>
       <c r="K62" t="s">
         <v>66</v>
@@ -3510,19 +3507,19 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B63" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C63" t="s">
         <v>9</v>
       </c>
       <c r="D63" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E63" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F63" t="s">
         <v>8</v>
@@ -3542,19 +3539,19 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B64" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C64" t="s">
         <v>9</v>
       </c>
       <c r="D64" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E64" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F64" t="s">
         <v>8</v>
@@ -3574,19 +3571,19 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C65" t="s">
         <v>9</v>
       </c>
       <c r="D65" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E65" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F65" t="s">
         <v>8</v>
@@ -3606,19 +3603,19 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B66" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C66" t="s">
         <v>9</v>
       </c>
       <c r="D66" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E66" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F66" t="s">
         <v>8</v>
@@ -3638,19 +3635,19 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B67" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C67" t="s">
         <v>9</v>
       </c>
       <c r="D67" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E67" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F67" t="s">
         <v>8</v>
@@ -3670,19 +3667,19 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B68" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C68" t="s">
         <v>9</v>
       </c>
       <c r="D68" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E68" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F68" t="s">
         <v>8</v>
@@ -3702,19 +3699,19 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B69" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C69" t="s">
         <v>9</v>
       </c>
       <c r="D69" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E69" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F69" t="s">
         <v>8</v>
@@ -3734,19 +3731,19 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="B70" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
       <c r="C70" t="s">
         <v>9</v>
       </c>
       <c r="D70" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="E70" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
       <c r="F70" t="s">
         <v>8</v>
@@ -3766,19 +3763,19 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="B71" t="s">
-        <v>250</v>
+        <v>278</v>
       </c>
       <c r="C71" t="s">
         <v>9</v>
       </c>
       <c r="D71" t="s">
-        <v>259</v>
+        <v>281</v>
       </c>
       <c r="E71" t="s">
-        <v>250</v>
+        <v>278</v>
       </c>
       <c r="F71" t="s">
         <v>8</v>
@@ -3798,19 +3795,19 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="B72" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
       <c r="C72" t="s">
         <v>9</v>
       </c>
       <c r="D72" t="s">
-        <v>288</v>
+        <v>259</v>
       </c>
       <c r="E72" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
       <c r="F72" t="s">
         <v>8</v>
@@ -3822,10 +3819,7 @@
         <v>194</v>
       </c>
       <c r="I72" s="4">
-        <v>45474</v>
-      </c>
-      <c r="J72" t="s">
-        <v>287</v>
+        <v>45444</v>
       </c>
       <c r="K72" t="s">
         <v>66</v>
@@ -3841,8 +3835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD4EC6B-F420-4E98-B717-46E4AD07ABBC}">
   <dimension ref="A1:A68"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection sqref="A1:A68"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4112,22 +4106,22 @@
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>285</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>43</v>
+        <v>295</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.35">
@@ -4191,31 +4185,73 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A68">
-    <sortCondition ref="A1:A68"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A67">
+    <sortCondition ref="A1:A67"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
-    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
-    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
-      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
-      <Description>63P7TJYCZHM3-28990658-16955</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -4491,77 +4527,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
+    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
+    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
+      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
+      <Description>63P7TJYCZHM3-28990658-16955</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
-    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4580,18 +4579,13 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
+    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Remove 'Marine' rows from Terrestrial (NVIS) crosswalk.
</commit_message>
<xml_diff>
--- a/crosswalks/NVIS-IUCNGET/Terrestrial_IUCNGET.xlsx
+++ b/crosswalks/NVIS-IUCNGET/Terrestrial_IUCNGET.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu240\Downloads\ext\ecosystem-typology\crosswalks\NVIS-IUCNGET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fishe\Dropbox\Documents\NEAP\Ecosystem-Typology\crosswalks\NVIS-IUCNGET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92C44B3-C6D0-4076-99A9-75A65F986F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7049201B-7707-4235-A851-ED6338A151BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="11" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="274">
   <si>
     <t>MFT1.3 Coastal saltmarshes and reedbeds</t>
   </si>
@@ -810,60 +810,6 @@
     <t>M1.8 Subtidal mud plains</t>
   </si>
   <si>
-    <t>get:groups/M1.1</t>
-  </si>
-  <si>
-    <t>get:groups/M1.10</t>
-  </si>
-  <si>
-    <t>get:groups/M1.2</t>
-  </si>
-  <si>
-    <t>get:groups/M1.3</t>
-  </si>
-  <si>
-    <t>get:groups/M1.4</t>
-  </si>
-  <si>
-    <t>get:groups/M1.5</t>
-  </si>
-  <si>
-    <t>get:groups/M1.6</t>
-  </si>
-  <si>
-    <t>get:groups/M1.7</t>
-  </si>
-  <si>
-    <t>get:groups/M1.8</t>
-  </si>
-  <si>
-    <t>terr:M1.1_Seagrass_meadows</t>
-  </si>
-  <si>
-    <t>terr:M1.2_Kelp_forests</t>
-  </si>
-  <si>
-    <t>terr:M1.3_Photic_coral_reefs</t>
-  </si>
-  <si>
-    <t>terr:M1.4_Shellfish_beds_and_reefs</t>
-  </si>
-  <si>
-    <t>terr:M1.5_Photo-limited_marine_animal_forests</t>
-  </si>
-  <si>
-    <t>terr:M1.6_Subtidal_rocky_reefs</t>
-  </si>
-  <si>
-    <t>terr:M1.7_Subtidal_sand_beds</t>
-  </si>
-  <si>
-    <t>terr:M1.8_Subtidal_mud_plains</t>
-  </si>
-  <si>
-    <t>terr:M1.10_Rhodolith_Maërl_beds</t>
-  </si>
-  <si>
     <t>F2.4 Freeze-thaw freshwater lakes</t>
   </si>
   <si>
@@ -879,16 +825,10 @@
     <t>get:groups/MT2.2</t>
   </si>
   <si>
-    <t>get:groups/M1.9</t>
-  </si>
-  <si>
     <t>terr:F2.4_Freeze-thaw_freshwater_lakes</t>
   </si>
   <si>
     <t>terr:MT2.2_Large_seabird_and_pinniped_colonies_</t>
-  </si>
-  <si>
-    <t>terr:M1.9_Upwelling_zones</t>
   </si>
   <si>
     <t>terr:T4.4a_Semi_arid_woodlands</t>
@@ -1059,9 +999,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1099,7 +1039,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1205,7 +1145,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1347,7 +1287,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1361,62 +1301,62 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="104.21875" customWidth="1"/>
+    <col min="1" max="1" width="104.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -1428,33 +1368,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564BC65A-26C0-42CC-8916-F0F3B4195637}">
-  <dimension ref="A1:Q72"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63:XFD72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" customWidth="1"/>
-    <col min="5" max="5" width="50.21875" customWidth="1"/>
-    <col min="6" max="6" width="29.21875" customWidth="1"/>
+    <col min="2" max="2" width="50.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="50.28515625" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" customWidth="1"/>
     <col min="7" max="8" width="34" customWidth="1"/>
-    <col min="9" max="9" width="11.77734375" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
     <col min="12" max="12" width="34" customWidth="1"/>
-    <col min="13" max="13" width="35.77734375" customWidth="1"/>
-    <col min="14" max="14" width="34.44140625" customWidth="1"/>
-    <col min="15" max="15" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.77734375" customWidth="1"/>
-    <col min="17" max="17" width="57.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.7109375" customWidth="1"/>
+    <col min="14" max="14" width="34.42578125" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" customWidth="1"/>
+    <col min="17" max="17" width="57.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>68</v>
       </c>
@@ -1503,7 +1443,7 @@
       <c r="P1" s="5"/>
       <c r="Q1"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -1537,7 +1477,7 @@
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -1571,7 +1511,7 @@
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -1605,7 +1545,7 @@
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1639,7 +1579,7 @@
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1673,7 +1613,7 @@
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>88</v>
       </c>
@@ -1706,7 +1646,7 @@
       </c>
       <c r="P7" s="3"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>89</v>
       </c>
@@ -1739,7 +1679,7 @@
       </c>
       <c r="P8" s="3"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>90</v>
       </c>
@@ -1772,7 +1712,7 @@
       </c>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>91</v>
       </c>
@@ -1805,21 +1745,21 @@
       </c>
       <c r="P10" s="3"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>280</v>
+        <v>261</v>
       </c>
       <c r="B11" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="E11" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
@@ -1838,7 +1778,7 @@
       </c>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>92</v>
       </c>
@@ -1871,7 +1811,7 @@
       </c>
       <c r="P12" s="3"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -1904,7 +1844,7 @@
       </c>
       <c r="P13" s="3"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -1937,7 +1877,7 @@
       </c>
       <c r="P14" s="3"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -1970,7 +1910,7 @@
       </c>
       <c r="P15" s="3"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>96</v>
       </c>
@@ -2003,7 +1943,7 @@
       </c>
       <c r="P16" s="3"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>97</v>
       </c>
@@ -2036,7 +1976,7 @@
       </c>
       <c r="P17" s="3"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>98</v>
       </c>
@@ -2069,7 +2009,7 @@
       </c>
       <c r="P18" s="3"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2102,7 +2042,7 @@
       </c>
       <c r="P19" s="3"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>100</v>
       </c>
@@ -2135,7 +2075,7 @@
       </c>
       <c r="P20" s="3"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>101</v>
       </c>
@@ -2168,7 +2108,7 @@
       </c>
       <c r="P21" s="3"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -2188,10 +2128,10 @@
         <v>8</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="H22" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
       <c r="I22" s="4">
         <v>45512</v>
@@ -2201,7 +2141,7 @@
       </c>
       <c r="P22" s="3"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -2234,7 +2174,7 @@
       </c>
       <c r="P23" s="3"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -2267,7 +2207,7 @@
       </c>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -2300,7 +2240,7 @@
       </c>
       <c r="P25" s="3"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>106</v>
       </c>
@@ -2333,7 +2273,7 @@
       </c>
       <c r="P26" s="3"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -2366,7 +2306,7 @@
       </c>
       <c r="P27" s="3"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -2399,7 +2339,7 @@
       </c>
       <c r="P28" s="3"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>109</v>
       </c>
@@ -2432,21 +2372,21 @@
       </c>
       <c r="P29" s="3"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
       <c r="B30" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="C30" t="s">
         <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="E30" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="F30" t="s">
         <v>8</v>
@@ -2465,7 +2405,7 @@
       </c>
       <c r="P30" s="3"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -2498,7 +2438,7 @@
       </c>
       <c r="P31" s="3"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>111</v>
       </c>
@@ -2531,7 +2471,7 @@
       </c>
       <c r="P32" s="3"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>112</v>
       </c>
@@ -2564,7 +2504,7 @@
       </c>
       <c r="P33" s="3"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>113</v>
       </c>
@@ -2597,27 +2537,27 @@
       </c>
       <c r="P34" s="3"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B35" s="7" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
       </c>
       <c r="D35" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="E35" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
       <c r="F35" t="s">
         <v>8</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="H35" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
       <c r="I35" s="4">
         <v>45504</v>
@@ -2627,7 +2567,7 @@
       </c>
       <c r="P35" s="3"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>114</v>
       </c>
@@ -2660,7 +2600,7 @@
       </c>
       <c r="P36" s="3"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>115</v>
       </c>
@@ -2693,7 +2633,7 @@
       </c>
       <c r="P37" s="3"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>116</v>
       </c>
@@ -2726,7 +2666,7 @@
       </c>
       <c r="P38" s="3"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>117</v>
       </c>
@@ -2759,7 +2699,7 @@
       </c>
       <c r="P39" s="3"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>118</v>
       </c>
@@ -2792,7 +2732,7 @@
       </c>
       <c r="P40" s="3"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>119</v>
       </c>
@@ -2825,7 +2765,7 @@
       </c>
       <c r="P41" s="3"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>120</v>
       </c>
@@ -2858,7 +2798,7 @@
       </c>
       <c r="P42" s="3"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>121</v>
       </c>
@@ -2891,7 +2831,7 @@
       </c>
       <c r="P43" s="3"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>122</v>
       </c>
@@ -2924,7 +2864,7 @@
       </c>
       <c r="P44" s="3"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>123</v>
       </c>
@@ -2957,7 +2897,7 @@
       </c>
       <c r="P45" s="3"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>124</v>
       </c>
@@ -2990,7 +2930,7 @@
       </c>
       <c r="P46" s="3"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>125</v>
       </c>
@@ -3023,30 +2963,30 @@
       </c>
       <c r="P47" s="3"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
       <c r="B48" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="C48" t="s">
         <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="E48" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="F48" t="s">
         <v>8</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="H48" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
       <c r="I48" s="4">
         <v>45505</v>
@@ -3055,7 +2995,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>126</v>
       </c>
@@ -3088,7 +3028,7 @@
       </c>
       <c r="P49" s="3"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>127</v>
       </c>
@@ -3121,7 +3061,7 @@
       </c>
       <c r="P50" s="3"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>128</v>
       </c>
@@ -3153,7 +3093,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>129</v>
       </c>
@@ -3185,7 +3125,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>130</v>
       </c>
@@ -3217,7 +3157,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>131</v>
       </c>
@@ -3249,7 +3189,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>132</v>
       </c>
@@ -3281,27 +3221,27 @@
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B56" s="7" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
       <c r="C56" t="s">
         <v>9</v>
       </c>
       <c r="D56" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
       <c r="F56" t="s">
         <v>8</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="H56" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
       <c r="I56" s="4">
         <v>45504</v>
@@ -3310,7 +3250,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>133</v>
       </c>
@@ -3342,7 +3282,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>134</v>
       </c>
@@ -3374,7 +3314,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>135</v>
       </c>
@@ -3406,7 +3346,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>136</v>
       </c>
@@ -3438,7 +3378,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>137</v>
       </c>
@@ -3470,352 +3410,32 @@
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B62" s="7" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
       <c r="C62" t="s">
         <v>9</v>
       </c>
       <c r="D62" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
       <c r="F62" t="s">
         <v>8</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="H62" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
       <c r="I62" s="4">
         <v>45504</v>
       </c>
       <c r="K62" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>265</v>
-      </c>
-      <c r="B63" t="s">
-        <v>247</v>
-      </c>
-      <c r="C63" t="s">
-        <v>9</v>
-      </c>
-      <c r="D63" t="s">
-        <v>256</v>
-      </c>
-      <c r="E63" t="s">
-        <v>247</v>
-      </c>
-      <c r="F63" t="s">
-        <v>8</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H63" t="s">
-        <v>193</v>
-      </c>
-      <c r="I63" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K63" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>266</v>
-      </c>
-      <c r="B64" t="s">
-        <v>249</v>
-      </c>
-      <c r="C64" t="s">
-        <v>9</v>
-      </c>
-      <c r="D64" t="s">
-        <v>258</v>
-      </c>
-      <c r="E64" t="s">
-        <v>249</v>
-      </c>
-      <c r="F64" t="s">
-        <v>8</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H64" t="s">
-        <v>193</v>
-      </c>
-      <c r="I64" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K64" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>267</v>
-      </c>
-      <c r="B65" t="s">
-        <v>250</v>
-      </c>
-      <c r="C65" t="s">
-        <v>9</v>
-      </c>
-      <c r="D65" t="s">
-        <v>259</v>
-      </c>
-      <c r="E65" t="s">
-        <v>250</v>
-      </c>
-      <c r="F65" t="s">
-        <v>8</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H65" t="s">
-        <v>193</v>
-      </c>
-      <c r="I65" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K65" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>268</v>
-      </c>
-      <c r="B66" t="s">
-        <v>251</v>
-      </c>
-      <c r="C66" t="s">
-        <v>9</v>
-      </c>
-      <c r="D66" t="s">
-        <v>260</v>
-      </c>
-      <c r="E66" t="s">
-        <v>251</v>
-      </c>
-      <c r="F66" t="s">
-        <v>8</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H66" t="s">
-        <v>193</v>
-      </c>
-      <c r="I66" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K66" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>269</v>
-      </c>
-      <c r="B67" t="s">
-        <v>252</v>
-      </c>
-      <c r="C67" t="s">
-        <v>9</v>
-      </c>
-      <c r="D67" t="s">
-        <v>261</v>
-      </c>
-      <c r="E67" t="s">
-        <v>252</v>
-      </c>
-      <c r="F67" t="s">
-        <v>8</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H67" t="s">
-        <v>193</v>
-      </c>
-      <c r="I67" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K67" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>270</v>
-      </c>
-      <c r="B68" t="s">
-        <v>253</v>
-      </c>
-      <c r="C68" t="s">
-        <v>9</v>
-      </c>
-      <c r="D68" t="s">
-        <v>262</v>
-      </c>
-      <c r="E68" t="s">
-        <v>253</v>
-      </c>
-      <c r="F68" t="s">
-        <v>8</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H68" t="s">
-        <v>193</v>
-      </c>
-      <c r="I68" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K68" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>271</v>
-      </c>
-      <c r="B69" t="s">
-        <v>254</v>
-      </c>
-      <c r="C69" t="s">
-        <v>9</v>
-      </c>
-      <c r="D69" t="s">
-        <v>263</v>
-      </c>
-      <c r="E69" t="s">
-        <v>254</v>
-      </c>
-      <c r="F69" t="s">
-        <v>8</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H69" t="s">
-        <v>193</v>
-      </c>
-      <c r="I69" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K69" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>272</v>
-      </c>
-      <c r="B70" t="s">
-        <v>255</v>
-      </c>
-      <c r="C70" t="s">
-        <v>9</v>
-      </c>
-      <c r="D70" t="s">
-        <v>264</v>
-      </c>
-      <c r="E70" t="s">
-        <v>255</v>
-      </c>
-      <c r="F70" t="s">
-        <v>8</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H70" t="s">
-        <v>193</v>
-      </c>
-      <c r="I70" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K70" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>282</v>
-      </c>
-      <c r="B71" t="s">
-        <v>276</v>
-      </c>
-      <c r="C71" t="s">
-        <v>9</v>
-      </c>
-      <c r="D71" t="s">
-        <v>279</v>
-      </c>
-      <c r="E71" t="s">
-        <v>276</v>
-      </c>
-      <c r="F71" t="s">
-        <v>8</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H71" t="s">
-        <v>193</v>
-      </c>
-      <c r="I71" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K71" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>273</v>
-      </c>
-      <c r="B72" t="s">
-        <v>248</v>
-      </c>
-      <c r="C72" t="s">
-        <v>9</v>
-      </c>
-      <c r="D72" t="s">
-        <v>257</v>
-      </c>
-      <c r="E72" t="s">
-        <v>248</v>
-      </c>
-      <c r="F72" t="s">
-        <v>8</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H72" t="s">
-        <v>193</v>
-      </c>
-      <c r="I72" s="4">
-        <v>45444</v>
-      </c>
-      <c r="K72" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3833,347 +3453,347 @@
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>56</v>
       </c>
@@ -4187,82 +3807,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
-    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
-    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
-      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
-      <Description>63P7TJYCZHM3-28990658-16955</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -4538,34 +4082,83 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
+    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
+    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
+      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
+      <Description>63P7TJYCZHM3-28990658-16955</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
-    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4582,4 +4175,31 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
+    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>